<commit_message>
Let me try that again. Big update: complete overhaul of event_generator.py and nuc_reaction.py. Both now use relativistic 4-vectors consistently to track frame changes coherently. Also implemented two decay options: a realistic mode (3y cascade for gamma and Maxwellian emission for neutron) + a max_emission_mode (single step decay for both). Both decay functions now are correctly boosted between frames. Also implemented 4 neutron emission. Finally, the regime of 1 and 2 kinematic solutions are now correctly identified and robustly handled based on the kinematics.
</commit_message>
<xml_diff>
--- a/ReacInfoFiles/Qi_dipole-old_ESR_std.xlsx
+++ b/ReacInfoFiles/Qi_dipole-old_ESR_std.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leckenby\Documents\NECTAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\G4bl_simulations\NECTAR_G4bl_Sim\Code\ReacInfoFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0114D8-88B9-4ED9-BF0D-816B08491899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5588549-A368-4E21-8BA3-1B90230D6B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GPAC" sheetId="7" r:id="rId1"/>
@@ -771,7 +771,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="2">
-        <v>82</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>204.97448196438955</v>
+        <v>238.05078783332203</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>20</v>
       </c>
       <c r="B7" s="4">
-        <v>13</v>
+        <v>17.239999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -796,7 +796,7 @@
       </c>
       <c r="B8" s="4">
         <f>SQRT((B7*B6+B6*931.5)^2-(931.5*B6)^2)</f>
-        <v>32010.163370423787</v>
+        <v>42859.282631582784</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -805,7 +805,7 @@
       </c>
       <c r="B9" s="4">
         <f>$B$8/(2.997925*100*$B$5)</f>
-        <v>1.3021267909663445</v>
+        <v>1.5539473727147792</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
       </c>
       <c r="B11" s="6">
         <f>B9/B10</f>
-        <v>0.20483353641125443</v>
+        <v>0.24444665293609866</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -930,7 +930,7 @@
       </c>
       <c r="B26" s="21">
         <f>B14*B19*$B$9</f>
-        <v>-0.66470425698803481</v>
+        <v>-0.79325257797079107</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -939,7 +939,7 @@
       </c>
       <c r="B27" s="22">
         <f>B15*B20*$B$9</f>
-        <v>0.59838951513091143</v>
+        <v>0.71411311198633054</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -948,7 +948,7 @@
       </c>
       <c r="B28" s="22">
         <f>B16*B21*$B$9</f>
-        <v>0.43855995696524031</v>
+        <v>0.5233738355066655</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -957,7 +957,7 @@
       </c>
       <c r="B29" s="22">
         <f>B17*B22*$B$9</f>
-        <v>-0.59301513133727168</v>
+        <v>-0.70769936669360867</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -966,7 +966,7 @@
       </c>
       <c r="B30" s="23">
         <f>B18*B23*$B$9</f>
-        <v>0.54855405763416343</v>
+        <v>0.65463988804042061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>